<commit_message>
fix: correct loan import template when downloading
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-loan-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-loan-template.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lambert\accupay\AccuPay\ImportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="En9ae2sejJZaCVelsS9fXuwI807AoEu5Vss2v2v8Pnw13WAZdRMqVvSlyws6058VJ/9GckHarG5wbIOL3SVYFg==" workbookSaltValue="Ma8I2FeAOTakd1YKqf3pTQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19890" windowHeight="8355" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="1" r:id="rId1"/>
-    <sheet name="Options" sheetId="2" r:id="rId2"/>
+    <sheet name="Options" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -398,18 +399,18 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="89.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="3" customWidth="1"/>
+    <col min="6" max="7" width="17.28515625" style="3" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" style="3" customWidth="1"/>
     <col min="9" max="9" width="60.5703125" style="3" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" style="3" customWidth="1"/>
@@ -454,7 +455,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="iNBocmw5dxyyrN05Dc0wjnEVVYoA061oKxiVk9fLr77wuaZ/8YT/4PC5X7Y4VxY/od1KvqfVytXe4mjm/3Px0A==" saltValue="p+BwovY9eos/aih7und6Yw==" spinCount="100000" sheet="1" objects="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="l9zznDD/0DWZl5GITtPhX7tFIknYdZF0M7uaOhS71GV+wIQ3zjGqcrrB/SiJPTKCnXxGlMBX4B5qVypB9T6G+g==" saltValue="TWrRvmpcp4MNHfEvogLIIg==" spinCount="100000" sheet="1" objects="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576">
       <formula1>"Per pay period,End of the month,First half"</formula1>
@@ -488,7 +489,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>